<commit_message>
Implement balance analysis endpoints and update requirements; add PDF processing logic and Excel integration
</commit_message>
<xml_diff>
--- a/static/files/analise_balanco_modelo.xlsx
+++ b/static/files/analise_balanco_modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Falcão\Desktop\Development\vector-datasheet-automation-backend\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DE080A-3C1E-4B48-8FE9-87C635C71CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D59127-8849-42FC-B0B2-A23DFDB2F166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="103">
   <si>
     <t>ANÁLISE DE EMPRESAS ( REV 3 - 19 AGO 2024 )</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>EMPRESA</t>
-  </si>
-  <si>
-    <t>MODELO VER 3 - 19AGO2024</t>
   </si>
   <si>
     <t>BALANÇO/BALANCETE</t>
@@ -916,7 +913,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -999,24 +996,9 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1126,40 +1108,43 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1168,6 +1153,24 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1491,17 +1494,17 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.59765625" style="70" customWidth="1"/>
-    <col min="2" max="5" width="17.59765625" style="70" customWidth="1"/>
-    <col min="6" max="6" width="2.09765625" style="70" customWidth="1"/>
-    <col min="7" max="7" width="31.8984375" style="70" customWidth="1"/>
-    <col min="8" max="8" width="64" style="70" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="14.09765625" style="70" customWidth="1"/>
+    <col min="1" max="1" width="44.59765625" style="65" customWidth="1"/>
+    <col min="2" max="5" width="17.59765625" style="65" customWidth="1"/>
+    <col min="6" max="6" width="2.09765625" style="65" customWidth="1"/>
+    <col min="7" max="7" width="31.8984375" style="65" customWidth="1"/>
+    <col min="8" max="8" width="64" style="65" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="14.09765625" style="65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1518,41 +1521,39 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="92" t="s">
+      <c r="B3" s="94"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="64"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E4" s="69">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="69"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="E4" s="74">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="96" t="s">
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="100"/>
+      <c r="G5" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="98"/>
-      <c r="G5" s="93" t="s">
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="97"/>
+      <c r="M5" s="101" t="s">
         <v>5</v>
-      </c>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="99" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="1" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="28">
         <v>44561</v>
@@ -1564,636 +1565,571 @@
         <v>45291</v>
       </c>
       <c r="E6" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="H6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="38">
+      <c r="I6" s="33">
         <f>B6</f>
         <v>44561</v>
       </c>
-      <c r="J6" s="39">
+      <c r="J6" s="34">
         <f>C6</f>
         <v>44926</v>
       </c>
-      <c r="K6" s="38">
+      <c r="K6" s="33">
         <f>D6</f>
         <v>45291</v>
       </c>
-      <c r="L6" s="38" t="str">
+      <c r="L6" s="33" t="str">
         <f>E6</f>
         <v>30/06/2024</v>
       </c>
-      <c r="M6" s="100"/>
+      <c r="M6" s="102"/>
     </row>
     <row r="7" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="82"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="75"/>
-      <c r="C7" s="30">
-        <v>14677170</v>
-      </c>
-      <c r="D7" s="30">
-        <v>28782758</v>
-      </c>
-      <c r="E7" s="30"/>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="70" t="e">
+        <f>(B15+B20)/B21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="70" t="e">
+        <f>(C15+C20)/C21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K7" s="70" t="e">
+        <f>(D15+D20)/D21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L7" s="70" t="e">
+        <f>(E15+E20)/E21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="71" t="s">
         <v>13</v>
-      </c>
-      <c r="I7" s="76" t="e">
-        <f>(B15+B20)/B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J7" s="76">
-        <f>(C15+C20)/C21</f>
-        <v>2.0441301463081976</v>
-      </c>
-      <c r="K7" s="76">
-        <f>(D15+D20)/D21</f>
-        <v>4.68117939299316</v>
-      </c>
-      <c r="L7" s="76" t="e">
-        <f>(E15+E20)/E21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M7" s="77" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="83"/>
+      <c r="C8" s="87"/>
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="33">
-        <v>268961</v>
-      </c>
-      <c r="D8" s="33">
-        <v>248358</v>
-      </c>
-      <c r="E8" s="33"/>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="76" t="e">
+      <c r="I8" s="70" t="e">
         <f>B15/B19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="70" t="e">
         <f>C15/C19</f>
-        <v>3.2949130751247697</v>
-      </c>
-      <c r="K8" s="76">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="70" t="e">
         <f>D15/D19</f>
-        <v>3.2521553862149188</v>
-      </c>
-      <c r="L8" s="76" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" s="70" t="e">
         <f>E15/E19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="77" t="s">
-        <v>14</v>
+      <c r="M8" s="71" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="87"/>
-      <c r="C9" s="33">
-        <v>10011027</v>
-      </c>
-      <c r="D9" s="33">
-        <v>22473903</v>
-      </c>
-      <c r="E9" s="33"/>
+        <v>17</v>
+      </c>
+      <c r="B9" s="83"/>
+      <c r="C9" s="87"/>
+      <c r="D9" s="87"/>
+      <c r="E9" s="87"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="70" t="e">
+        <f>B13/B21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="70" t="e">
+        <f>C13/C21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="70" t="e">
+        <f>D13/D21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L9" s="70" t="e">
+        <f>E13/E21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="71" t="s">
         <v>20</v>
-      </c>
-      <c r="I9" s="76" t="e">
-        <f>B13/B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J9" s="76">
-        <f>C13/C21</f>
-        <v>0.96778510934226225</v>
-      </c>
-      <c r="K9" s="76">
-        <f>D13/D21</f>
-        <v>1.2452502647377246</v>
-      </c>
-      <c r="L9" s="76" t="e">
-        <f>E13/E21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M9" s="77" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="83"/>
+      <c r="C10" s="87"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="87"/>
-      <c r="C10" s="33">
-        <v>6642105</v>
-      </c>
-      <c r="D10" s="33">
-        <v>16204417</v>
-      </c>
-      <c r="E10" s="33"/>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="70" t="e">
+        <f>'DRE e CICLO'!B17/'DRE e CICLO'!B9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="70" t="e">
+        <f>'DRE e CICLO'!D17/'DRE e CICLO'!D9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="70" t="e">
+        <f>'DRE e CICLO'!F17/'DRE e CICLO'!F9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L10" s="70" t="e">
+        <f>'DRE e CICLO'!H17/'DRE e CICLO'!H9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" s="71" t="s">
         <v>24</v>
-      </c>
-      <c r="I10" s="76" t="e">
-        <f>'DRE e CICLO'!B17/'DRE e CICLO'!B9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J10" s="76" t="e">
-        <f>'DRE e CICLO'!D17/'DRE e CICLO'!D9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="76" t="e">
-        <f>'DRE e CICLO'!F17/'DRE e CICLO'!F9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L10" s="76" t="e">
-        <f>'DRE e CICLO'!H17/'DRE e CICLO'!H9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M10" s="77" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="83"/>
+      <c r="C11" s="87"/>
+      <c r="D11" s="87"/>
+      <c r="E11" s="87"/>
+      <c r="G11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="87"/>
-      <c r="C11" s="33">
-        <v>366813</v>
-      </c>
-      <c r="D11" s="33">
-        <v>620275</v>
-      </c>
-      <c r="E11" s="33"/>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="70" t="e">
+        <f>'DRE e CICLO'!B17/'COMPARATIVO BALANÇO'!B21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="70" t="e">
+        <f>'DRE e CICLO'!D17/'COMPARATIVO BALANÇO'!C21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="70" t="e">
+        <f>'DRE e CICLO'!F17/'COMPARATIVO BALANÇO'!D21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L11" s="70" t="e">
+        <f>'DRE e CICLO'!H17/'COMPARATIVO BALANÇO'!E21</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="71" t="s">
         <v>28</v>
-      </c>
-      <c r="I11" s="76" t="e">
-        <f>'DRE e CICLO'!B17/'COMPARATIVO BALANÇO'!B21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J11" s="76">
-        <f>'DRE e CICLO'!D17/'COMPARATIVO BALANÇO'!C21</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="76">
-        <f>'DRE e CICLO'!F17/'COMPARATIVO BALANÇO'!D21</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="76" t="e">
-        <f>'DRE e CICLO'!H17/'COMPARATIVO BALANÇO'!E21</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M11" s="77" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="83"/>
+      <c r="C12" s="87"/>
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="87"/>
-      <c r="C12" s="33">
-        <v>2930134</v>
-      </c>
-      <c r="D12" s="33">
-        <v>6173355</v>
-      </c>
-      <c r="E12" s="33"/>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="70" t="e">
+        <f>(B9+B13)/(B15+B20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" s="70" t="e">
+        <f>(C9+C13)/(C15+C20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K12" s="70" t="e">
+        <f>(D9+D13)/(D15+D20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L12" s="70" t="e">
+        <f>(E9+E13)/(E15+E20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="71" t="s">
         <v>32</v>
-      </c>
-      <c r="I12" s="76" t="e">
-        <f>(B9+B13)/(B15+B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J12" s="76">
-        <f>(C9+C13)/(C15+C20)</f>
-        <v>1.4892056417278765</v>
-      </c>
-      <c r="K12" s="76">
-        <f>(D9+D13)/(D15+D20)</f>
-        <v>1.2136213795815667</v>
-      </c>
-      <c r="L12" s="76" t="e">
-        <f>(E9+E13)/(E15+E20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="77" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="83"/>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="G13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="87"/>
-      <c r="C13" s="33">
-        <v>4666143</v>
-      </c>
-      <c r="D13" s="33">
-        <v>6308855</v>
-      </c>
-      <c r="E13" s="33"/>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="70" t="e">
+        <f>B9/B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="70" t="e">
+        <f>C9/C15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K13" s="70" t="e">
+        <f>D9/D15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" s="70" t="e">
+        <f>E9/E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M13" s="71" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="I13" s="76" t="e">
-        <f>B9/B15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J13" s="76">
-        <f>C9/C15</f>
-        <v>1.1482383002678069</v>
-      </c>
-      <c r="K13" s="76">
-        <f>D9/D15</f>
-        <v>1.2198287564499388</v>
-      </c>
-      <c r="L13" s="76" t="e">
-        <f>E9/E15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M13" s="77" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="B14" s="84"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="G14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="88"/>
-      <c r="C14" s="32">
-        <v>14677170</v>
-      </c>
-      <c r="D14" s="32">
-        <v>28782758</v>
-      </c>
-      <c r="E14" s="32"/>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="70" t="e">
+        <f>(B9-B12)/B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J14" s="70" t="e">
+        <f>(C9-C12)/C15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="70" t="e">
+        <f>(D9-D12)/D15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L14" s="70" t="e">
+        <f>(E9-E12)/E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" s="71" t="s">
         <v>39</v>
-      </c>
-      <c r="I14" s="76" t="e">
-        <f>(B9-B12)/B15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J14" s="76">
-        <f>(C9-C12)/C15</f>
-        <v>0.81215968578430686</v>
-      </c>
-      <c r="K14" s="76">
-        <f>(D9-D12)/D15</f>
-        <v>0.88475407214726065</v>
-      </c>
-      <c r="L14" s="76" t="e">
-        <f>(E9-E12)/E15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M14" s="77" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="85"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="89"/>
+      <c r="G15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="89"/>
-      <c r="C15" s="34">
-        <v>8718597</v>
-      </c>
-      <c r="D15" s="34">
-        <v>18423818</v>
-      </c>
-      <c r="E15" s="34"/>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="70" t="e">
+        <f>B8/B15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J15" s="70" t="e">
+        <f>C8/C15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="70" t="e">
+        <f>D8/D15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="70" t="e">
+        <f>E8/E15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="71" t="s">
         <v>43</v>
-      </c>
-      <c r="I15" s="76" t="e">
-        <f>B8/B15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J15" s="76">
-        <f>C8/C15</f>
-        <v>3.0849114828911121E-2</v>
-      </c>
-      <c r="K15" s="76">
-        <f>D8/D15</f>
-        <v>1.348026777077368E-2</v>
-      </c>
-      <c r="L15" s="76" t="e">
-        <f>E8/E15</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="77" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="85"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="89"/>
+      <c r="G16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="89"/>
-      <c r="C16" s="34">
-        <v>5834009</v>
-      </c>
-      <c r="D16" s="34">
-        <v>12529945</v>
-      </c>
-      <c r="E16" s="34"/>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="70" t="e">
+        <f>B9/(B15+B20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J16" s="70" t="e">
+        <f>C9/(C15+C20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K16" s="70" t="e">
+        <f>D9/(D15+D20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" s="70" t="e">
+        <f>E9/(E15+E20)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="71" t="s">
         <v>47</v>
-      </c>
-      <c r="I16" s="76" t="e">
-        <f>B9/(B15+B20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J16" s="76">
-        <f>C9/(C15+C20)</f>
-        <v>1.015759706257412</v>
-      </c>
-      <c r="K16" s="76">
-        <f>D9/(D15+D20)</f>
-        <v>0.94760930010398281</v>
-      </c>
-      <c r="L16" s="76" t="e">
-        <f>E9/(E15+E20)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="77" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="85"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="G17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="34">
-        <v>182234</v>
-      </c>
-      <c r="D17" s="34">
-        <v>60253</v>
-      </c>
-      <c r="E17" s="34"/>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="I17" s="70" t="e">
+        <f>(B15+B20)/B7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="70" t="e">
+        <f>(C15+C20)/C7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="70" t="e">
+        <f>(D15+D20)/D7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="70" t="e">
+        <f>(E15+E20)/E7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="71" t="s">
         <v>51</v>
-      </c>
-      <c r="I17" s="76" t="e">
-        <f>(B15+B20)/B7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J17" s="76">
-        <f>(C15+C20)/C7</f>
-        <v>0.67149893337748356</v>
-      </c>
-      <c r="K17" s="76">
-        <f>(D15+D20)/D7</f>
-        <v>0.82398021065250249</v>
-      </c>
-      <c r="L17" s="76" t="e">
-        <f>(E15+E20)/E7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M17" s="77" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="85"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="G18" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="34">
-        <v>56276</v>
-      </c>
-      <c r="D18" s="34">
-        <v>168510</v>
-      </c>
-      <c r="E18" s="34"/>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="70" t="e">
+        <f>(B15+B20)/'DRE e CICLO'!B13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J18" s="70" t="e">
+        <f>(C15+C20)/'DRE e CICLO'!D13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K18" s="70" t="e">
+        <f>(D15+D20)/'DRE e CICLO'!F13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="70" t="e">
+        <f>(E15+E20)/'DRE e CICLO'!H13</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="71" t="s">
         <v>55</v>
-      </c>
-      <c r="I18" s="76" t="e">
-        <f>(B15+B20)/'DRE e CICLO'!B13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="76" t="e">
-        <f>(C15+C20)/'DRE e CICLO'!D13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="76" t="e">
-        <f>(D15+D20)/'DRE e CICLO'!F13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="76" t="e">
-        <f>(E15+E20)/'DRE e CICLO'!H13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M18" s="77" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="85"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="G19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="89"/>
-      <c r="C19" s="35">
-        <f>C15-C16-C17-C18</f>
-        <v>2646078</v>
-      </c>
-      <c r="D19" s="35">
-        <f>D15-D16-D17-D18</f>
-        <v>5665110</v>
-      </c>
-      <c r="E19" s="35">
-        <f>E15-E16-E17-E18</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="78">
+      <c r="I19" s="35"/>
+      <c r="J19" s="72">
         <f>B11+'DRE e CICLO'!D10*-1-'COMPARATIVO BALANÇO'!C11</f>
-        <v>-366813</v>
-      </c>
-      <c r="K19" s="78">
+        <v>0</v>
+      </c>
+      <c r="K19" s="72">
         <f>C11+'DRE e CICLO'!F10*-1-'COMPARATIVO BALANÇO'!D11</f>
-        <v>-253462</v>
-      </c>
-      <c r="L19" s="78">
+        <v>0</v>
+      </c>
+      <c r="L19" s="72">
         <f>D11+'DRE e CICLO'!H10*-1-'COMPARATIVO BALANÇO'!E11</f>
-        <v>620275</v>
+        <v>0</v>
       </c>
       <c r="M19" s="21"/>
     </row>
     <row r="20" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="89"/>
-      <c r="C20" s="34">
-        <v>1137107</v>
-      </c>
-      <c r="D20" s="34">
-        <v>5292605</v>
-      </c>
-      <c r="E20" s="34"/>
+        <v>59</v>
+      </c>
+      <c r="B20" s="85"/>
+      <c r="C20" s="89"/>
+      <c r="D20" s="89"/>
+      <c r="E20" s="89"/>
     </row>
     <row r="21" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="85"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="89"/>
+    </row>
+    <row r="22" spans="1:13" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="73"/>
+    </row>
+    <row r="23" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="89"/>
-      <c r="C21" s="34">
-        <v>4821466</v>
-      </c>
-      <c r="D21" s="34">
-        <v>5066335</v>
-      </c>
-      <c r="E21" s="34"/>
-    </row>
-    <row r="22" spans="1:13" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G22" s="79"/>
-    </row>
-    <row r="23" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="41" t="str">
+      <c r="B23" s="36" t="str">
         <f>IF(B9+B13=B7,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
-      <c r="C23" s="41" t="str">
+      <c r="C23" s="36" t="str">
         <f>IF(C9+C13=C7,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
-      <c r="D23" s="41" t="str">
+      <c r="D23" s="36" t="str">
         <f>IF(D9+D13=D7,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
-      <c r="E23" s="41" t="str">
+      <c r="E23" s="36" t="str">
         <f>IF(E9+E13=E7,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
     </row>
     <row r="24" spans="1:13" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="74">
+        <f>B7-(B9+B13)</f>
+        <v>0</v>
+      </c>
+      <c r="C24" s="74">
+        <f>C7-(C9+C13)</f>
+        <v>0</v>
+      </c>
+      <c r="D24" s="74">
+        <f>D7-(D9+D13)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="74">
+        <f>E7-(E9+E13)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="80">
-        <f>B7-(B9+B13)</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="80">
-        <f>C7-(C9+C13)</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="80">
-        <f>D7-(D9+D13)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="80">
-        <f>E7-(E9+E13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="41" t="str">
+      <c r="B25" s="36" t="str">
         <f>IF(B7=B15+B20+B21,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
-      <c r="C25" s="41" t="str">
+      <c r="C25" s="36" t="str">
         <f>IF(C7=C15+C20+C21,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
-      <c r="D25" s="41" t="str">
+      <c r="D25" s="36" t="str">
         <f>IF(D7=D15+D20+D21,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
-      <c r="E25" s="42" t="str">
+      <c r="E25" s="37" t="str">
         <f>IF(E7=E15+E20+E21,"CERTO","ERRADO")</f>
         <v>CERTO</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B26" s="80">
+        <v>64</v>
+      </c>
+      <c r="B26" s="74">
         <f>B7-(B15+B20+B21)</f>
         <v>0</v>
       </c>
-      <c r="C26" s="80">
+      <c r="C26" s="74">
         <f>C7-(C15+C20+C21)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="80">
+      <c r="D26" s="74">
         <f>D7-(D15+D20+D21)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="81">
+      <c r="E26" s="75">
         <f>E7-(E15+E20+E21)</f>
         <v>0</v>
       </c>
@@ -2208,9 +2144,9 @@
     <row r="34" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
-      <c r="C34" s="90"/>
-      <c r="D34" s="91"/>
-      <c r="E34" s="69"/>
+      <c r="C34" s="92"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="64"/>
     </row>
     <row r="35" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14"/>
@@ -2258,15 +2194,15 @@
       <c r="A41" s="14"/>
       <c r="B41" s="14"/>
       <c r="C41" s="13"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="14"/>
       <c r="B42" s="14"/>
       <c r="C42" s="13"/>
-      <c r="D42" s="83"/>
-      <c r="E42" s="83"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="77"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="14"/>
@@ -2298,25 +2234,25 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38" style="70" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" style="70" customWidth="1"/>
-    <col min="4" max="4" width="16.59765625" style="70" customWidth="1"/>
-    <col min="6" max="6" width="16.59765625" style="70" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="70" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.59765625" style="70" customWidth="1"/>
-    <col min="10" max="10" width="1.59765625" style="70" customWidth="1"/>
-    <col min="11" max="11" width="39.19921875" style="70" customWidth="1"/>
-    <col min="12" max="15" width="16.59765625" style="70" customWidth="1"/>
+    <col min="1" max="1" width="38" style="65" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" style="65" customWidth="1"/>
+    <col min="4" max="4" width="16.59765625" style="65" customWidth="1"/>
+    <col min="6" max="6" width="16.59765625" style="65" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="65" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.59765625" style="65" customWidth="1"/>
+    <col min="10" max="10" width="1.59765625" style="65" customWidth="1"/>
+    <col min="11" max="11" width="39.19921875" style="65" customWidth="1"/>
+    <col min="12" max="15" width="16.59765625" style="65" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2329,12 +2265,12 @@
         <f>'COMPARATIVO BALANÇO'!A3</f>
         <v>EMPRESA</v>
       </c>
-      <c r="B3" s="92" t="str">
+      <c r="B3" s="94">
         <f>'COMPARATIVO BALANÇO'!B3</f>
-        <v>MODELO VER 3 - 19AGO2024</v>
-      </c>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
+        <v>0</v>
+      </c>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
     </row>
     <row r="4" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
@@ -2344,495 +2280,503 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="103">
+      <c r="H4" s="105">
         <f>'COMPARATIVO BALANÇO'!E4</f>
         <v>1000</v>
       </c>
-      <c r="I4" s="94"/>
+      <c r="I4" s="96"/>
     </row>
     <row r="5" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="102" t="s">
+      <c r="A5" s="104" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="99"/>
+      <c r="F5" s="99"/>
+      <c r="G5" s="99"/>
+      <c r="H5" s="99"/>
+      <c r="I5" s="100"/>
+      <c r="K5" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="97"/>
-      <c r="H5" s="97"/>
-      <c r="I5" s="98"/>
-      <c r="K5" s="96" t="s">
-        <v>68</v>
-      </c>
-      <c r="L5" s="97"/>
-      <c r="M5" s="97"/>
-      <c r="N5" s="97"/>
-      <c r="O5" s="98"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="99"/>
+      <c r="N5" s="99"/>
+      <c r="O5" s="100"/>
     </row>
     <row r="6" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="72"/>
-      <c r="B6" s="101">
+      <c r="A6" s="67"/>
+      <c r="B6" s="103">
         <f>'COMPARATIVO BALANÇO'!B6</f>
         <v>44561</v>
       </c>
-      <c r="C6" s="98"/>
-      <c r="D6" s="101">
+      <c r="C6" s="100"/>
+      <c r="D6" s="103">
         <f>'COMPARATIVO BALANÇO'!C6</f>
         <v>44926</v>
       </c>
-      <c r="E6" s="98"/>
-      <c r="F6" s="101">
+      <c r="E6" s="100"/>
+      <c r="F6" s="103">
         <f>'COMPARATIVO BALANÇO'!D6</f>
         <v>45291</v>
       </c>
-      <c r="G6" s="98"/>
-      <c r="H6" s="101" t="str">
+      <c r="G6" s="100"/>
+      <c r="H6" s="103" t="str">
         <f>'COMPARATIVO BALANÇO'!E6</f>
         <v>30/06/2024</v>
       </c>
-      <c r="I6" s="98"/>
-      <c r="K6" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="L6" s="36">
+      <c r="I6" s="100"/>
+      <c r="K6" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="L6" s="31">
         <f>B6</f>
         <v>44561</v>
       </c>
-      <c r="M6" s="36">
+      <c r="M6" s="31">
         <f>D6</f>
         <v>44926</v>
       </c>
-      <c r="N6" s="36">
+      <c r="N6" s="31">
         <f>F6</f>
         <v>45291</v>
       </c>
-      <c r="O6" s="36" t="str">
+      <c r="O6" s="31" t="str">
         <f>H6</f>
         <v>30/06/2024</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="C7" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="D7" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="H7" s="71" t="s">
-        <v>71</v>
-      </c>
-      <c r="I7" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="L7" s="50" t="e">
+      <c r="L7" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!B10/B9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M7" s="50" t="e">
+      <c r="M7" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!C10/D9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N7" s="50" t="e">
+      <c r="N7" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!D10/F9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O7" s="50" t="e">
+      <c r="O7" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!E10/H9)*360</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="78" t="e">
+        <f t="shared" ref="C8:C17" si="0">B8/$B$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D8" s="90"/>
+      <c r="E8" s="78" t="e">
+        <f t="shared" ref="E8:E17" si="1">D8/$D$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="90"/>
+      <c r="G8" s="78" t="e">
+        <f t="shared" ref="G8:G17" si="2">F8/$F$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="79"/>
+      <c r="I8" s="78" t="e">
+        <f t="shared" ref="I8:I17" si="3">H8/$H$9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="84" t="e">
-        <f t="shared" ref="C8:C17" si="0">B8/$B$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="84" t="e">
-        <f t="shared" ref="E8:E17" si="1">D8/$D$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="84" t="e">
-        <f t="shared" ref="G8:G17" si="2">F8/$F$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="84" t="e">
-        <f t="shared" ref="I8:I17" si="3">H8/$H$9</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="L8" s="50" t="e">
+      <c r="L8" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!B11/B9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M8" s="50" t="e">
+      <c r="M8" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!C11/D9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N8" s="50" t="e">
+      <c r="N8" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!D11/F9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O8" s="50" t="e">
+      <c r="O8" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!E11/H9)*360</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="78" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F9" s="90"/>
+      <c r="G9" s="78" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="78" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="84" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="84" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="84" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="L9" s="50" t="e">
+      <c r="L9" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!B16/B9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M9" s="50" t="e">
+      <c r="M9" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!C16/D9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N9" s="50" t="e">
+      <c r="N9" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!D16/F9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O9" s="50" t="e">
+      <c r="O9" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!E16/H9)*360</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D10" s="90"/>
+      <c r="E10" s="78" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F10" s="90"/>
+      <c r="G10" s="78" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="78" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K10" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="84" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="84" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="84" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="L10" s="50" t="e">
+      <c r="L10" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!B17/B9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M10" s="50" t="e">
+      <c r="M10" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!C17/D9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N10" s="50" t="e">
+      <c r="N10" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!D17/F9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O10" s="50" t="e">
+      <c r="O10" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!E17/H9)*360</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D11" s="90"/>
+      <c r="E11" s="78" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F11" s="90"/>
+      <c r="G11" s="78" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="78" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K11" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="84" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="84" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="84" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" s="50" t="e">
+      <c r="L11" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!B18/B9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M11" s="50" t="e">
+      <c r="M11" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!C18/D9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N11" s="50" t="e">
+      <c r="N11" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!D18/F9)*360</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O11" s="50" t="e">
+      <c r="O11" s="45" t="e">
         <f>('COMPARATIVO BALANÇO'!E18/H9)*360</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="4">
+        <v>0</v>
+      </c>
+      <c r="C12" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="78" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
+      </c>
+      <c r="G12" s="78" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="78" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="84" t="e">
+      <c r="L12" s="46" t="e">
+        <f>L7+L8-L9-L10-L11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="46" t="e">
+        <f>M7+M8-M9-M10-M11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" s="46" t="e">
+        <f>N7+N8-N9-N10-N11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O12" s="46" t="e">
+        <f>O7+O8-O9-O10-O11</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="42">
+        <f>B9+B10+B11+B12</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="80" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="84" t="e">
+      <c r="D13" s="42">
+        <f>D9+D10+D11+D12</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="80" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="84" t="e">
+      <c r="F13" s="42">
+        <f>F9+F10+F11+F12</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="80" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="84" t="e">
+      <c r="H13" s="43">
+        <f>H9+H10+H11+H12</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="80" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="L12" s="51" t="e">
-        <f>L7+L8-L9-L10-L11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="51" t="e">
-        <f>M7+M8-M9-M10-M11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" s="51" t="e">
-        <f>N7+N8-N9-N10-N11</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O12" s="51" t="e">
-        <f>O7+O8-O9-O10-O11</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46" t="s">
+      <c r="K13" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="47">
-        <f>B9+B10+B11+B12</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="85" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D13" s="47">
-        <f>D9+D10+D11+D12</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="85" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F13" s="47">
-        <f>F9+F10+F11+F12</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="85" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H13" s="48">
-        <f>H9+H10+H11+H12</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="85" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="L13" s="86" t="e">
+      <c r="L13" s="81" t="e">
         <f>L12/360*B9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="86" t="e">
+      <c r="M13" s="81" t="e">
         <f>M12/360*D9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N13" s="86" t="e">
+      <c r="N13" s="81" t="e">
         <f>N12/360*F9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O13" s="86" t="e">
+      <c r="O13" s="81" t="e">
         <f>O12/360*H9</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D14" s="90"/>
+      <c r="E14" s="78" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F14" s="90"/>
+      <c r="G14" s="78" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H14" s="4"/>
+      <c r="I14" s="78" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="84" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="84" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="84" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="L14" s="86">
+      <c r="L14" s="81">
         <f>'COMPARATIVO BALANÇO'!B9-'COMPARATIVO BALANÇO'!B15</f>
         <v>0</v>
       </c>
-      <c r="M14" s="86">
+      <c r="M14" s="81">
         <f>'COMPARATIVO BALANÇO'!C9-'COMPARATIVO BALANÇO'!C15</f>
-        <v>1292430</v>
-      </c>
-      <c r="N14" s="86">
+        <v>0</v>
+      </c>
+      <c r="N14" s="81">
         <f>'COMPARATIVO BALANÇO'!D9-'COMPARATIVO BALANÇO'!D15</f>
-        <v>4050085</v>
-      </c>
-      <c r="O14" s="86">
+        <v>0</v>
+      </c>
+      <c r="O14" s="81">
         <f>'COMPARATIVO BALANÇO'!E9-'COMPARATIVO BALANÇO'!E15</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="78" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D15" s="90"/>
+      <c r="E15" s="78" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F15" s="90"/>
+      <c r="G15" s="78" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="78" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K15" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="84" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="84" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="84" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="84" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L15" s="86" t="e">
+      <c r="L15" s="81" t="e">
         <f>L14-L13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="86" t="e">
+      <c r="M15" s="81" t="e">
         <f>M14-M13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N15" s="86" t="e">
+      <c r="N15" s="81" t="e">
         <f>N14-N13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O15" s="86" t="e">
+      <c r="O15" s="81" t="e">
         <f>O14-O13</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B16" s="17">
         <f>B13+B14+B15</f>
         <v>0</v>
       </c>
-      <c r="C16" s="84" t="e">
+      <c r="C16" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2840,7 +2784,7 @@
         <f>D13+D14+D15</f>
         <v>0</v>
       </c>
-      <c r="E16" s="84" t="e">
+      <c r="E16" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -2848,7 +2792,7 @@
         <f>F13+F14+F15</f>
         <v>0</v>
       </c>
-      <c r="G16" s="84" t="e">
+      <c r="G16" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -2856,32 +2800,32 @@
         <f>H13+H14+H15</f>
         <v>0</v>
       </c>
-      <c r="I16" s="84" t="e">
+      <c r="I16" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" s="4"/>
-      <c r="C17" s="84" t="e">
+      <c r="C17" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="84" t="e">
+      <c r="D17" s="90"/>
+      <c r="E17" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="84" t="e">
+      <c r="F17" s="90"/>
+      <c r="G17" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="84" t="e">
+      <c r="I17" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
@@ -2891,16 +2835,16 @@
     </row>
     <row r="19" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="19"/>
-      <c r="F19" s="79"/>
-      <c r="H19" s="79"/>
+      <c r="F19" s="73"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
-      <c r="F20" s="79"/>
+      <c r="F20" s="73"/>
     </row>
     <row r="21" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="20"/>
-      <c r="F21" s="79"/>
+      <c r="F21" s="73"/>
     </row>
     <row r="22" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="20"/>
@@ -2915,13 +2859,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K5:O5"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -2935,34 +2879,34 @@
   </sheetPr>
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.8984375" style="73" customWidth="1"/>
-    <col min="2" max="2" width="20.69921875" style="73" customWidth="1"/>
-    <col min="3" max="3" width="2.69921875" style="73" customWidth="1"/>
-    <col min="4" max="4" width="20.69921875" style="73" customWidth="1"/>
-    <col min="5" max="5" width="2.69921875" style="73" customWidth="1"/>
-    <col min="6" max="6" width="20.69921875" style="73" customWidth="1"/>
-    <col min="7" max="7" width="2.69921875" style="73" customWidth="1"/>
-    <col min="8" max="8" width="20.69921875" style="73" customWidth="1"/>
-    <col min="9" max="9" width="2.69921875" style="73" customWidth="1"/>
-    <col min="10" max="10" width="20.69921875" style="73" customWidth="1"/>
-    <col min="11" max="20" width="8.8984375" style="73" customWidth="1"/>
-    <col min="21" max="16384" width="8.8984375" style="73"/>
+    <col min="1" max="1" width="10.8984375" style="68" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" style="68" customWidth="1"/>
+    <col min="3" max="3" width="2.69921875" style="68" customWidth="1"/>
+    <col min="4" max="4" width="20.69921875" style="68" customWidth="1"/>
+    <col min="5" max="5" width="2.69921875" style="68" customWidth="1"/>
+    <col min="6" max="6" width="20.69921875" style="68" customWidth="1"/>
+    <col min="7" max="7" width="2.69921875" style="68" customWidth="1"/>
+    <col min="8" max="8" width="20.69921875" style="68" customWidth="1"/>
+    <col min="9" max="9" width="2.69921875" style="68" customWidth="1"/>
+    <col min="10" max="10" width="20.69921875" style="68" customWidth="1"/>
+    <col min="11" max="37" width="8.8984375" style="68" customWidth="1"/>
+    <col min="38" max="16384" width="8.8984375" style="68"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B1" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B2" s="52" t="s">
-        <v>92</v>
+      <c r="B2" s="47" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
@@ -2970,112 +2914,112 @@
         <f>'COMPARATIVO BALANÇO'!A3</f>
         <v>EMPRESA</v>
       </c>
-      <c r="C3" s="104" t="str">
+      <c r="C3" s="106">
         <f>'DRE e CICLO'!B3</f>
-        <v>MODELO VER 3 - 19AGO2024</v>
-      </c>
-      <c r="D3" s="105"/>
-      <c r="E3" s="105"/>
+        <v>0</v>
+      </c>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B5" s="53" t="s">
-        <v>93</v>
+      <c r="B5" s="48" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="23"/>
     </row>
     <row r="7" spans="1:14" ht="24.6" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="54">
-        <v>0</v>
-      </c>
-      <c r="D7" s="57">
-        <v>0</v>
-      </c>
-      <c r="F7" s="60">
-        <v>0</v>
-      </c>
-      <c r="H7" s="63">
-        <v>0</v>
-      </c>
-      <c r="J7" s="66">
+      <c r="B7" s="49">
+        <v>0</v>
+      </c>
+      <c r="D7" s="52">
+        <v>0</v>
+      </c>
+      <c r="F7" s="55">
+        <v>0</v>
+      </c>
+      <c r="H7" s="58">
+        <v>0</v>
+      </c>
+      <c r="J7" s="61">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="50" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="58" t="s">
+      <c r="F8" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="F8" s="61" t="s">
+      <c r="H8" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="J8" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="H8" s="64" t="s">
-        <v>84</v>
-      </c>
-      <c r="J8" s="67" t="s">
-        <v>97</v>
-      </c>
     </row>
     <row r="9" spans="1:14" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="56"/>
-      <c r="D9" s="59"/>
-      <c r="F9" s="62"/>
-      <c r="H9" s="65"/>
-      <c r="J9" s="68"/>
+      <c r="B9" s="51"/>
+      <c r="D9" s="54"/>
+      <c r="F9" s="57"/>
+      <c r="H9" s="60"/>
+      <c r="J9" s="63"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:14" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="D15" s="58">
+        <v>0</v>
+      </c>
+      <c r="F15" s="55">
+        <v>0</v>
+      </c>
+      <c r="H15" s="52">
+        <v>0</v>
+      </c>
+      <c r="J15" s="49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="D15" s="63">
-        <v>0</v>
-      </c>
-      <c r="F15" s="60">
-        <v>0</v>
-      </c>
-      <c r="H15" s="57">
-        <v>0</v>
-      </c>
-      <c r="J15" s="54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="43.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="67" t="s">
+      <c r="D16" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="56" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="F16" s="61" t="s">
+      <c r="H16" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="H16" s="58" t="s">
+      <c r="J16" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="J16" s="55" t="s">
-        <v>103</v>
-      </c>
     </row>
     <row r="17" spans="1:12" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B17" s="68"/>
+      <c r="B17" s="63"/>
       <c r="C17" s="25"/>
-      <c r="D17" s="65"/>
+      <c r="D17" s="60"/>
       <c r="E17" s="25"/>
-      <c r="F17" s="62"/>
+      <c r="F17" s="57"/>
       <c r="G17" s="25"/>
-      <c r="H17" s="59"/>
-      <c r="J17" s="56"/>
+      <c r="H17" s="54"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="26"/>

</xml_diff>

<commit_message>
Refactor balance analysis logic to use template and output paths; update Excel handling and improve error management
</commit_message>
<xml_diff>
--- a/static/files/analise_balanco_modelo.xlsx
+++ b/static/files/analise_balanco_modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Falcão\Desktop\Development\vector-datasheet-automation-backend\static\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D59127-8849-42FC-B0B2-A23DFDB2F166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FE9C3B-CE1B-4F76-ADB9-F4B9EFF6D1CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -913,7 +913,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1133,9 +1133,6 @@
     <xf numFmtId="167" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="167" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1193,14 +1190,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1494,7 +1491,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1521,9 +1518,9 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
       <c r="E3" s="64"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1532,22 +1529,22 @@
       </c>
     </row>
     <row r="5" spans="1:13" s="1" customFormat="1" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="100"/>
-      <c r="G5" s="95" t="s">
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="99"/>
+      <c r="G5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="97"/>
-      <c r="M5" s="101" t="s">
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="100" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1589,16 +1586,16 @@
         <f>E6</f>
         <v>30/06/2024</v>
       </c>
-      <c r="M6" s="102"/>
+      <c r="M6" s="101"/>
     </row>
     <row r="7" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="85"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
       <c r="G7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1629,10 +1626,10 @@
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1663,10 +1660,10 @@
       <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
         <v>18</v>
@@ -1698,10 +1695,10 @@
       <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
       <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1732,10 +1729,10 @@
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
       <c r="G11" s="2" t="s">
         <v>26</v>
       </c>
@@ -1766,10 +1763,10 @@
       <c r="A12" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="83"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="87"/>
-      <c r="E12" s="87"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
       <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
@@ -1800,10 +1797,10 @@
       <c r="A13" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="83"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="87"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
       <c r="G13" s="2" t="s">
         <v>34</v>
       </c>
@@ -1834,10 +1831,10 @@
       <c r="A14" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="84"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="88"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
       <c r="G14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1868,10 +1865,10 @@
       <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="85"/>
-      <c r="C15" s="89"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
+      <c r="B15" s="84"/>
+      <c r="C15" s="88"/>
+      <c r="D15" s="88"/>
+      <c r="E15" s="88"/>
       <c r="G15" s="2" t="s">
         <v>41</v>
       </c>
@@ -1902,10 +1899,10 @@
       <c r="A16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="89"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
+      <c r="B16" s="84"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="88"/>
+      <c r="E16" s="88"/>
       <c r="G16" s="2" t="s">
         <v>45</v>
       </c>
@@ -1936,10 +1933,10 @@
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="85"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
+      <c r="B17" s="84"/>
+      <c r="C17" s="88"/>
+      <c r="D17" s="88"/>
+      <c r="E17" s="88"/>
       <c r="G17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1970,10 +1967,10 @@
       <c r="A18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="85"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="88"/>
+      <c r="D18" s="88"/>
+      <c r="E18" s="88"/>
       <c r="G18" s="2" t="s">
         <v>53</v>
       </c>
@@ -2004,10 +2001,22 @@
       <c r="A19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="85"/>
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
+      <c r="B19" s="84">
+        <f>B15-B16-B17-B18</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="84">
+        <f>C15-C16-C17-C18</f>
+        <v>0</v>
+      </c>
+      <c r="D19" s="84">
+        <f>D15-D16-D17-D18</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="84">
+        <f>E15-E16-E17-E18</f>
+        <v>0</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>57</v>
       </c>
@@ -2033,19 +2042,19 @@
       <c r="A20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="85"/>
-      <c r="C20" s="89"/>
-      <c r="D20" s="89"/>
-      <c r="E20" s="89"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="88"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="88"/>
     </row>
     <row r="21" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="85"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="89"/>
+      <c r="B21" s="84"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="90"/>
+      <c r="E21" s="88"/>
     </row>
     <row r="22" spans="1:13" ht="24.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G22" s="73"/>
@@ -2144,8 +2153,8 @@
     <row r="34" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14"/>
       <c r="B34" s="14"/>
-      <c r="C34" s="92"/>
-      <c r="D34" s="93"/>
+      <c r="C34" s="91"/>
+      <c r="D34" s="92"/>
       <c r="E34" s="64"/>
     </row>
     <row r="35" spans="1:5" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -2233,8 +2242,8 @@
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2265,12 +2274,12 @@
         <f>'COMPARATIVO BALANÇO'!A3</f>
         <v>EMPRESA</v>
       </c>
-      <c r="B3" s="94">
+      <c r="B3" s="93">
         <f>'COMPARATIVO BALANÇO'!B3</f>
         <v>0</v>
       </c>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
     </row>
     <row r="4" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15"/>
@@ -2280,31 +2289,31 @@
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
-      <c r="H4" s="105">
+      <c r="H4" s="102">
         <f>'COMPARATIVO BALANÇO'!E4</f>
         <v>1000</v>
       </c>
-      <c r="I4" s="96"/>
+      <c r="I4" s="95"/>
     </row>
     <row r="5" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="104" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
-      <c r="H5" s="99"/>
-      <c r="I5" s="100"/>
-      <c r="K5" s="98" t="s">
+      <c r="B5" s="98"/>
+      <c r="C5" s="98"/>
+      <c r="D5" s="98"/>
+      <c r="E5" s="98"/>
+      <c r="F5" s="98"/>
+      <c r="G5" s="98"/>
+      <c r="H5" s="98"/>
+      <c r="I5" s="99"/>
+      <c r="K5" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="L5" s="99"/>
-      <c r="M5" s="99"/>
-      <c r="N5" s="99"/>
-      <c r="O5" s="100"/>
+      <c r="L5" s="98"/>
+      <c r="M5" s="98"/>
+      <c r="N5" s="98"/>
+      <c r="O5" s="99"/>
     </row>
     <row r="6" spans="1:15" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="67"/>
@@ -2312,22 +2321,22 @@
         <f>'COMPARATIVO BALANÇO'!B6</f>
         <v>44561</v>
       </c>
-      <c r="C6" s="100"/>
+      <c r="C6" s="99"/>
       <c r="D6" s="103">
         <f>'COMPARATIVO BALANÇO'!C6</f>
         <v>44926</v>
       </c>
-      <c r="E6" s="100"/>
+      <c r="E6" s="99"/>
       <c r="F6" s="103">
         <f>'COMPARATIVO BALANÇO'!D6</f>
         <v>45291</v>
       </c>
-      <c r="G6" s="100"/>
+      <c r="G6" s="99"/>
       <c r="H6" s="103" t="str">
         <f>'COMPARATIVO BALANÇO'!E6</f>
         <v>30/06/2024</v>
       </c>
-      <c r="I6" s="100"/>
+      <c r="I6" s="99"/>
       <c r="K6" s="44" t="s">
         <v>68</v>
       </c>
@@ -2400,22 +2409,22 @@
       <c r="A8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="89"/>
       <c r="C8" s="78" t="e">
         <f t="shared" ref="C8:C17" si="0">B8/$B$9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D8" s="90"/>
+      <c r="D8" s="89"/>
       <c r="E8" s="78" t="e">
         <f t="shared" ref="E8:E17" si="1">D8/$D$9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F8" s="90"/>
+      <c r="F8" s="89"/>
       <c r="G8" s="78" t="e">
         <f t="shared" ref="G8:G17" si="2">F8/$F$9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="H8" s="79"/>
+      <c r="H8" s="89"/>
       <c r="I8" s="78" t="e">
         <f t="shared" ref="I8:I17" si="3">H8/$H$9</f>
         <v>#DIV/0!</v>
@@ -2444,22 +2453,22 @@
       <c r="A9" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="4"/>
+      <c r="B9" s="89"/>
       <c r="C9" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="89"/>
       <c r="E9" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F9" s="90"/>
+      <c r="F9" s="89"/>
       <c r="G9" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="89"/>
       <c r="I9" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -2488,22 +2497,22 @@
       <c r="A10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="89"/>
       <c r="C10" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D10" s="90"/>
+      <c r="D10" s="89"/>
       <c r="E10" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F10" s="90"/>
+      <c r="F10" s="89"/>
       <c r="G10" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="89"/>
       <c r="I10" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -2532,22 +2541,22 @@
       <c r="A11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="89"/>
       <c r="C11" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D11" s="90"/>
+      <c r="D11" s="89"/>
       <c r="E11" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F11" s="90"/>
+      <c r="F11" s="89"/>
       <c r="G11" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="89"/>
       <c r="I11" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -2632,7 +2641,7 @@
         <f>B9+B10+B11+B12</f>
         <v>0</v>
       </c>
-      <c r="C13" s="80" t="e">
+      <c r="C13" s="79" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
@@ -2640,7 +2649,7 @@
         <f>D9+D10+D11+D12</f>
         <v>0</v>
       </c>
-      <c r="E13" s="80" t="e">
+      <c r="E13" s="79" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
@@ -2648,7 +2657,7 @@
         <f>F9+F10+F11+F12</f>
         <v>0</v>
       </c>
-      <c r="G13" s="80" t="e">
+      <c r="G13" s="79" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -2656,26 +2665,26 @@
         <f>H9+H10+H11+H12</f>
         <v>0</v>
       </c>
-      <c r="I13" s="80" t="e">
+      <c r="I13" s="79" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="81" t="e">
+      <c r="L13" s="80" t="e">
         <f>L12/360*B9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M13" s="81" t="e">
+      <c r="M13" s="80" t="e">
         <f>M12/360*D9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N13" s="81" t="e">
+      <c r="N13" s="80" t="e">
         <f>N12/360*F9</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O13" s="81" t="e">
+      <c r="O13" s="80" t="e">
         <f>O12/360*H9</f>
         <v>#DIV/0!</v>
       </c>
@@ -2684,22 +2693,22 @@
       <c r="A14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="4"/>
+      <c r="B14" s="89"/>
       <c r="C14" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D14" s="90"/>
+      <c r="D14" s="89"/>
       <c r="E14" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F14" s="90"/>
+      <c r="F14" s="89"/>
       <c r="G14" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="89"/>
       <c r="I14" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -2707,19 +2716,19 @@
       <c r="K14" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="L14" s="81">
+      <c r="L14" s="80">
         <f>'COMPARATIVO BALANÇO'!B9-'COMPARATIVO BALANÇO'!B15</f>
         <v>0</v>
       </c>
-      <c r="M14" s="81">
+      <c r="M14" s="80">
         <f>'COMPARATIVO BALANÇO'!C9-'COMPARATIVO BALANÇO'!C15</f>
         <v>0</v>
       </c>
-      <c r="N14" s="81">
+      <c r="N14" s="80">
         <f>'COMPARATIVO BALANÇO'!D9-'COMPARATIVO BALANÇO'!D15</f>
         <v>0</v>
       </c>
-      <c r="O14" s="81">
+      <c r="O14" s="80">
         <f>'COMPARATIVO BALANÇO'!E9-'COMPARATIVO BALANÇO'!E15</f>
         <v>0</v>
       </c>
@@ -2728,22 +2737,22 @@
       <c r="A15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="4"/>
+      <c r="B15" s="89"/>
       <c r="C15" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D15" s="90"/>
+      <c r="D15" s="89"/>
       <c r="E15" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F15" s="90"/>
+      <c r="F15" s="89"/>
       <c r="G15" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="89"/>
       <c r="I15" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -2751,19 +2760,19 @@
       <c r="K15" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="L15" s="81" t="e">
+      <c r="L15" s="80" t="e">
         <f>L14-L13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M15" s="81" t="e">
+      <c r="M15" s="80" t="e">
         <f>M14-M13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="N15" s="81" t="e">
+      <c r="N15" s="80" t="e">
         <f>N14-N13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O15" s="81" t="e">
+      <c r="O15" s="80" t="e">
         <f>O14-O13</f>
         <v>#DIV/0!</v>
       </c>
@@ -2809,22 +2818,22 @@
       <c r="A17" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="4"/>
+      <c r="B17" s="89"/>
       <c r="C17" s="78" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="D17" s="90"/>
+      <c r="D17" s="89"/>
       <c r="E17" s="78" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="F17" s="90"/>
+      <c r="F17" s="89"/>
       <c r="G17" s="78" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="H17" s="4"/>
+      <c r="H17" s="89"/>
       <c r="I17" s="78" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -2859,13 +2868,13 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K5:O5"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" scale="52" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -2895,8 +2904,8 @@
     <col min="8" max="8" width="20.69921875" style="68" customWidth="1"/>
     <col min="9" max="9" width="2.69921875" style="68" customWidth="1"/>
     <col min="10" max="10" width="20.69921875" style="68" customWidth="1"/>
-    <col min="11" max="37" width="8.8984375" style="68" customWidth="1"/>
-    <col min="38" max="16384" width="8.8984375" style="68"/>
+    <col min="11" max="38" width="8.8984375" style="68" customWidth="1"/>
+    <col min="39" max="16384" width="8.8984375" style="68"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
@@ -2914,12 +2923,12 @@
         <f>'COMPARATIVO BALANÇO'!A3</f>
         <v>EMPRESA</v>
       </c>
-      <c r="C3" s="106">
+      <c r="C3" s="105">
         <f>'DRE e CICLO'!B3</f>
         <v>0</v>
       </c>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="106"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B5" s="48" t="s">

</xml_diff>